<commit_message>
fix grammar errors in arsq xls
</commit_message>
<xml_diff>
--- a/Biomarkers/Supportfunctions/ARSQ.xlsx
+++ b/Biomarkers/Supportfunctions/ARSQ.xlsx
@@ -2739,10 +2739,10 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
       <selection pane="bottomRight" activeCell="D52" activeCellId="0" sqref="D52"/>
     </sheetView>
   </sheetViews>
@@ -2761,7 +2761,7 @@
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.53441295546559"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="11" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
compute ARSQ from GUI
</commit_message>
<xml_diff>
--- a/Biomarkers/Supportfunctions/ARSQ.xlsx
+++ b/Biomarkers/Supportfunctions/ARSQ.xlsx
@@ -694,7 +694,7 @@
     <t>Ich dachte in Bildern</t>
   </si>
   <si>
-    <t>jeg visualiserede mine tanker</t>
+    <t>Jeg visualiserede mine tanker</t>
   </si>
   <si>
     <t>Ho pensato per immagini</t>
@@ -2654,19 +2654,19 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Input" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Normal 2" xfId="22" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in 20% - Accent6" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in 20% - Accent4" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in 20% - Accent3" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Accent6" xfId="26" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Accent5" xfId="27" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Accent4" xfId="28" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Accent3" xfId="29" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Accent2" xfId="30" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Title" xfId="31" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Accent1" xfId="32" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Input" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Check Cell" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in 20% - Accent6" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in 20% - Accent4" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in 20% - Accent3" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Accent6" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Accent5" xfId="27" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Accent4" xfId="28" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Accent3" xfId="29" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Accent2" xfId="30" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Title" xfId="31" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Accent1" xfId="32" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2739,11 +2739,11 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
-      <selection pane="bottomRight" activeCell="D52" activeCellId="0" sqref="D52"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H56" activeCellId="0" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>